<commit_message>
Added connection to supabase
</commit_message>
<xml_diff>
--- a/assets/descriptions_engins.xlsx
+++ b/assets/descriptions_engins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bloom-fishing-form\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCE639E-1E10-4E0F-8B24-9D42089A96EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D3058F-BEBB-47AC-8A3A-9F0AD0B0BA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7248D41E-29AC-9D46-AA50-0A70CA5239B2}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$C$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$D$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>CHALUT DE FOND À PANNEAUX : filet en forme d'entonnoir traîné sur le fond marin. Des plaques en métal pouvant peser plusieurs tonnes chacunes se trouvent de chaque côté du filet, permettant de le garder ouvert, en contact avec le fond marin.</t>
   </si>
@@ -294,6 +294,90 @@
   </si>
   <si>
     <t>MANUAL BOTTOM GEARS : consist of a wide category including clamps, rakes, etc. Mostly used on shore or while diving, they are operated by arm power to catch animals leaving on the bottom, such as crustaceans, shells, algea, etc.</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>CASIER LANTERNE</t>
+  </si>
+  <si>
+    <t>SENNE TOURNANTE + DISPOSITIF DE CONCENTRATION DE POISSONS (DCP)</t>
+  </si>
+  <si>
+    <t>SENNE TOURNANTE</t>
+  </si>
+  <si>
+    <t>SENNE DE PLAGE</t>
+  </si>
+  <si>
+    <t>LIGNE VERTICALE</t>
+  </si>
+  <si>
+    <t>PALANGRE FIXE</t>
+  </si>
+  <si>
+    <t>ENGIN MANUEL DE FOND</t>
+  </si>
+  <si>
+    <t>POMPE</t>
+  </si>
+  <si>
+    <t>CHALUT PELAGIQUE</t>
+  </si>
+  <si>
+    <t>SENNE DEMERSALE</t>
+  </si>
+  <si>
+    <t>DRAGUE MECANIQUE</t>
+  </si>
+  <si>
+    <t>FILET RETOMBANT ou "EPERVIER"</t>
+  </si>
+  <si>
+    <t>FILET MAILLANT DERIVANT</t>
+  </si>
+  <si>
+    <t>FILET MAILLANT ANCRE ou "FIXE"</t>
+  </si>
+  <si>
+    <t>FILET TREMAIL</t>
+  </si>
+  <si>
+    <t>FILET SOULEVE MECANIQUE ou "FIXE"</t>
+  </si>
+  <si>
+    <t>FILET SOULEVE MANUEL OU "PORTABLE"</t>
+  </si>
+  <si>
+    <t>LIGNES ET CANNES MECANISEES</t>
+  </si>
+  <si>
+    <t>PALANGRE DERIVANTE</t>
+  </si>
+  <si>
+    <t>ENGIN MANUEL PELAGIQUE</t>
+  </si>
+  <si>
+    <t>PIEGE FIXE</t>
+  </si>
+  <si>
+    <t>PIEGE MOBILE</t>
+  </si>
+  <si>
+    <t>CHALUT DE FOND A PANNEAUX</t>
+  </si>
+  <si>
+    <t>CHALUT DE FOND A PERCHE</t>
+  </si>
+  <si>
+    <t>DRAGUE A MAIN</t>
+  </si>
+  <si>
+    <t>LIGNE A MAIN ou CANNE</t>
+  </si>
+  <si>
+    <t>LIGNE de TRAINE</t>
   </si>
 </sst>
 </file>
@@ -343,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,7 +438,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,413 +752,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE7467F-6651-FC4F-BC9F-16C10C72FBD0}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.19921875" style="4"/>
-    <col min="3" max="4" width="95.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="5" width="95.19921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:D1" xr:uid="{4DE7467F-6651-FC4F-BC9F-16C10C72FBD0}"/>
+  <autoFilter ref="D1:E1" xr:uid="{4DE7467F-6651-FC4F-BC9F-16C10C72FBD0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>